<commit_message>
Entered July 2025 Sulfide data and started plate QAQC (Still need to do plates 9 and 10)
</commit_message>
<xml_diff>
--- a/Porewater/Sulfide/Synoptic_CB/2025/July/202507_SampleList.xlsx
+++ b/Porewater/Sulfide/Synoptic_CB/2025/July/202507_SampleList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GlobalChangeEco\Porewater_R scripts &amp; Data\Data\Sulfide Microplate\COMPASS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/readz_si_edu1/Documents/synoptic-discrete-data/Porewater/Sulfide/Synoptic_CB/2025/July/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4487F391-0048-468E-BB20-574277D2E5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4487F391-0048-468E-BB20-574277D2E5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C2BF36F-79C5-4D90-8DE5-E4B2ADAE1B32}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{63E1FA8D-C94D-4A36-B1D4-6428EFA23086}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{63E1FA8D-C94D-4A36-B1D4-6428EFA23086}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>zone</t>
   </si>
   <si>
-    <t>Lys</t>
-  </si>
-  <si>
     <t>depth</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>GWI</t>
+  </si>
+  <si>
+    <t>replicate</t>
   </si>
 </sst>
 </file>
@@ -461,13 +461,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43B9C82-E323-4BD5-9979-8DDC9F7FD80F}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:A114"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,13 +481,13 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -518,16 +518,16 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -538,16 +538,16 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -564,10 +564,10 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -587,7 +587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -604,10 +604,10 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -621,13 +621,13 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -641,13 +641,13 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -661,13 +661,13 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -681,13 +681,13 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -701,13 +701,13 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -721,13 +721,13 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -738,16 +738,16 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
@@ -767,7 +767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -778,16 +778,16 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -798,16 +798,16 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -818,16 +818,16 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -838,16 +838,16 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -858,16 +858,16 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -878,16 +878,16 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -898,16 +898,16 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -918,13 +918,13 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
         <v>15</v>
       </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -935,13 +935,13 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -952,13 +952,13 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -966,19 +966,19 @@
         <v>202507</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
         <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -986,10 +986,10 @@
         <v>202507</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27" t="s">
         <v>3</v>
@@ -998,7 +998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1006,19 +1006,19 @@
         <v>202507</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1026,19 +1026,19 @@
         <v>202507</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1046,19 +1046,19 @@
         <v>202507</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1066,19 +1066,19 @@
         <v>202507</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1086,19 +1086,19 @@
         <v>202507</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1106,19 +1106,19 @@
         <v>202507</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1126,19 +1126,19 @@
         <v>202507</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>202507</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35" t="s">
         <v>2</v>
@@ -1155,10 +1155,10 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>202507</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
         <v>2</v>
@@ -1178,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>202507</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
         <v>2</v>
@@ -1195,10 +1195,10 @@
         <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1206,19 +1206,19 @@
         <v>202507</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1226,19 +1226,19 @@
         <v>202507</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1246,19 +1246,19 @@
         <v>202507</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1266,19 +1266,19 @@
         <v>202507</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1286,19 +1286,19 @@
         <v>202507</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1306,19 +1306,19 @@
         <v>202507</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E43" t="s">
         <v>3</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1326,10 +1326,10 @@
         <v>202507</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E44" t="s">
         <v>3</v>
@@ -1338,7 +1338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1346,19 +1346,19 @@
         <v>202507</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
       </c>
       <c r="F45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1366,19 +1366,19 @@
         <v>202507</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1386,19 +1386,19 @@
         <v>202507</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F47" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1406,19 +1406,19 @@
         <v>202507</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1426,19 +1426,19 @@
         <v>202507</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1446,16 +1446,16 @@
         <v>202507</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D50" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" t="s">
         <v>15</v>
       </c>
-      <c r="E50" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1463,16 +1463,16 @@
         <v>202507</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1480,16 +1480,16 @@
         <v>202507</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E52" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1497,10 +1497,10 @@
         <v>202507</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -1509,7 +1509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1517,19 +1517,19 @@
         <v>202507</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E54" t="s">
         <v>3</v>
       </c>
       <c r="F54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1537,19 +1537,19 @@
         <v>202507</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1557,19 +1557,19 @@
         <v>202507</v>
       </c>
       <c r="C56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F56" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1577,19 +1577,19 @@
         <v>202507</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1597,19 +1597,19 @@
         <v>202507</v>
       </c>
       <c r="C58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F58" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1617,19 +1617,19 @@
         <v>202507</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>202507</v>
       </c>
       <c r="C60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D60" t="s">
         <v>2</v>
@@ -1646,10 +1646,10 @@
         <v>3</v>
       </c>
       <c r="F60" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>202507</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D61" t="s">
         <v>2</v>
@@ -1669,7 +1669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1677,19 +1677,19 @@
         <v>202507</v>
       </c>
       <c r="C62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D62" t="s">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1697,19 +1697,19 @@
         <v>202507</v>
       </c>
       <c r="C63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F63" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1717,19 +1717,19 @@
         <v>202507</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D64" t="s">
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1737,19 +1737,19 @@
         <v>202507</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D65" t="s">
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1757,19 +1757,19 @@
         <v>202507</v>
       </c>
       <c r="C66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E66" t="s">
         <v>3</v>
       </c>
       <c r="F66" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1777,19 +1777,19 @@
         <v>202507</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F67" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1797,19 +1797,19 @@
         <v>202507</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F68" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1817,19 +1817,19 @@
         <v>202507</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F69" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1837,19 +1837,19 @@
         <v>202507</v>
       </c>
       <c r="C70" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1857,19 +1857,19 @@
         <v>202507</v>
       </c>
       <c r="C71" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E71" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F71" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1877,19 +1877,19 @@
         <v>202507</v>
       </c>
       <c r="C72" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F72" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1897,16 +1897,16 @@
         <v>202507</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D73" t="s">
+        <v>14</v>
+      </c>
+      <c r="E73" t="s">
         <v>15</v>
       </c>
-      <c r="E73" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1914,16 +1914,16 @@
         <v>202507</v>
       </c>
       <c r="C74" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E74" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1931,16 +1931,16 @@
         <v>202507</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E75" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1948,19 +1948,19 @@
         <v>202507</v>
       </c>
       <c r="C76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E76" t="s">
         <v>3</v>
       </c>
       <c r="F76" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1968,10 +1968,10 @@
         <v>202507</v>
       </c>
       <c r="C77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D77" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E77" t="s">
         <v>3</v>
@@ -1980,7 +1980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1988,19 +1988,19 @@
         <v>202507</v>
       </c>
       <c r="C78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E78" t="s">
         <v>3</v>
       </c>
       <c r="F78" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2008,19 +2008,19 @@
         <v>202507</v>
       </c>
       <c r="C79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F79" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2028,19 +2028,19 @@
         <v>202507</v>
       </c>
       <c r="C80" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D80" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F80" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2048,19 +2048,19 @@
         <v>202507</v>
       </c>
       <c r="C81" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F81" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2068,19 +2068,19 @@
         <v>202507</v>
       </c>
       <c r="C82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D82" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E82" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F82" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2088,19 +2088,19 @@
         <v>202507</v>
       </c>
       <c r="C83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D83" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E83" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F83" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2108,19 +2108,19 @@
         <v>202507</v>
       </c>
       <c r="C84" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D84" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E84" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F84" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2128,19 +2128,19 @@
         <v>202507</v>
       </c>
       <c r="C85" t="s">
+        <v>20</v>
+      </c>
+      <c r="D85" t="s">
         <v>21</v>
       </c>
-      <c r="D85" t="s">
-        <v>22</v>
-      </c>
       <c r="E85" t="s">
         <v>3</v>
       </c>
       <c r="F85" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2148,11 +2148,11 @@
         <v>202507</v>
       </c>
       <c r="C86" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86" t="s">
         <v>21</v>
       </c>
-      <c r="D86" t="s">
-        <v>22</v>
-      </c>
       <c r="E86" t="s">
         <v>3</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2168,19 +2168,19 @@
         <v>202507</v>
       </c>
       <c r="C87" t="s">
+        <v>20</v>
+      </c>
+      <c r="D87" t="s">
         <v>21</v>
       </c>
-      <c r="D87" t="s">
-        <v>22</v>
-      </c>
       <c r="E87" t="s">
         <v>3</v>
       </c>
       <c r="F87" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2188,19 +2188,19 @@
         <v>202507</v>
       </c>
       <c r="C88" t="s">
+        <v>20</v>
+      </c>
+      <c r="D88" t="s">
         <v>21</v>
       </c>
-      <c r="D88" t="s">
-        <v>22</v>
-      </c>
       <c r="E88" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F88" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2208,19 +2208,19 @@
         <v>202507</v>
       </c>
       <c r="C89" t="s">
+        <v>20</v>
+      </c>
+      <c r="D89" t="s">
         <v>21</v>
       </c>
-      <c r="D89" t="s">
-        <v>22</v>
-      </c>
       <c r="E89" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F89" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2228,19 +2228,19 @@
         <v>202507</v>
       </c>
       <c r="C90" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90" t="s">
         <v>21</v>
       </c>
-      <c r="D90" t="s">
-        <v>22</v>
-      </c>
       <c r="E90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F90" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2248,19 +2248,19 @@
         <v>202507</v>
       </c>
       <c r="C91" t="s">
+        <v>20</v>
+      </c>
+      <c r="D91" t="s">
         <v>21</v>
       </c>
-      <c r="D91" t="s">
-        <v>22</v>
-      </c>
       <c r="E91" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F91" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2268,19 +2268,19 @@
         <v>202507</v>
       </c>
       <c r="C92" t="s">
+        <v>20</v>
+      </c>
+      <c r="D92" t="s">
         <v>21</v>
       </c>
-      <c r="D92" t="s">
-        <v>22</v>
-      </c>
       <c r="E92" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F92" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2288,19 +2288,19 @@
         <v>202507</v>
       </c>
       <c r="C93" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" t="s">
         <v>21</v>
       </c>
-      <c r="D93" t="s">
-        <v>22</v>
-      </c>
       <c r="E93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F93" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>202507</v>
       </c>
       <c r="C94" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D94" t="s">
         <v>2</v>
@@ -2317,10 +2317,10 @@
         <v>3</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>202507</v>
       </c>
       <c r="C95" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D95" t="s">
         <v>2</v>
@@ -2340,7 +2340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>202507</v>
       </c>
       <c r="C96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D96" t="s">
         <v>2</v>
@@ -2357,10 +2357,10 @@
         <v>3</v>
       </c>
       <c r="F96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2368,19 +2368,19 @@
         <v>202507</v>
       </c>
       <c r="C97" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D97" t="s">
         <v>2</v>
       </c>
       <c r="E97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F97" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2388,19 +2388,19 @@
         <v>202507</v>
       </c>
       <c r="C98" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D98" t="s">
         <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F98" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2408,19 +2408,19 @@
         <v>202507</v>
       </c>
       <c r="C99" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D99" t="s">
         <v>2</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F99" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2428,19 +2428,19 @@
         <v>202507</v>
       </c>
       <c r="C100" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D100" t="s">
         <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2448,19 +2448,19 @@
         <v>202507</v>
       </c>
       <c r="C101" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F101" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2468,19 +2468,19 @@
         <v>202507</v>
       </c>
       <c r="C102" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F102" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2488,19 +2488,19 @@
         <v>202507</v>
       </c>
       <c r="C103" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D103" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E103" t="s">
         <v>3</v>
       </c>
       <c r="F103" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2508,10 +2508,10 @@
         <v>202507</v>
       </c>
       <c r="C104" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D104" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E104" t="s">
         <v>3</v>
@@ -2520,7 +2520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2528,19 +2528,19 @@
         <v>202507</v>
       </c>
       <c r="C105" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D105" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E105" t="s">
         <v>3</v>
       </c>
       <c r="F105" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2548,19 +2548,19 @@
         <v>202507</v>
       </c>
       <c r="C106" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D106" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F106" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2568,19 +2568,19 @@
         <v>202507</v>
       </c>
       <c r="C107" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D107" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F107" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2588,19 +2588,19 @@
         <v>202507</v>
       </c>
       <c r="C108" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D108" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F108" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2608,19 +2608,19 @@
         <v>202507</v>
       </c>
       <c r="C109" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D109" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E109" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F109" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2628,19 +2628,19 @@
         <v>202507</v>
       </c>
       <c r="C110" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D110" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E110" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F110" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2648,19 +2648,19 @@
         <v>202507</v>
       </c>
       <c r="C111" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E111" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F111" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2668,16 +2668,16 @@
         <v>202507</v>
       </c>
       <c r="C112" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D112" t="s">
+        <v>14</v>
+      </c>
+      <c r="E112" t="s">
         <v>15</v>
       </c>
-      <c r="E112" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2685,16 +2685,16 @@
         <v>202507</v>
       </c>
       <c r="C113" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E113" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2702,13 +2702,13 @@
         <v>202507</v>
       </c>
       <c r="C114" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D114" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E114" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>